<commit_message>
Fixed HHS Region Numbers
Fixed Problem with HHS Region Numbers
</commit_message>
<xml_diff>
--- a/HHSRegionsFile.xlsx
+++ b/HHSRegionsFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Github\MiscData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E9F98AA-EE94-441C-96E4-E0496D2EDF51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B92678-7EA4-48D5-87EE-9F546EB82036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD0F4EDB-3693-4E1A-AF17-48A6BE44BBF3}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="74">
   <si>
     <t>Connecticut</t>
   </si>
@@ -59,9 +59,6 @@
     <t>New York</t>
   </si>
   <si>
-    <t>U.S. Virgin Islands</t>
-  </si>
-  <si>
     <t>Region 2</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>Oklahoma</t>
   </si>
   <si>
-    <t>Texas exit</t>
-  </si>
-  <si>
     <t>Region 6</t>
   </si>
   <si>
@@ -249,6 +243,15 @@
   </si>
   <si>
     <t>HHSRegionNumber</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>Virgin Islands</t>
+  </si>
+  <si>
+    <t>Texas</t>
   </si>
 </sst>
 </file>
@@ -609,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DA0EDF-46AA-4D3A-9C46-6ACF23BD567A}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,16 +628,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -715,7 +718,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -726,13 +729,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -740,7 +743,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -754,13 +757,13 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -768,13 +771,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -782,13 +785,13 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -796,13 +799,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -810,13 +813,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -824,13 +827,13 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -838,13 +841,13 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -852,13 +855,13 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -866,13 +869,13 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -880,13 +883,13 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -894,13 +897,13 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -908,13 +911,13 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -922,13 +925,13 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -936,13 +939,13 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -950,13 +953,13 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -964,13 +967,13 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -978,13 +981,13 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -992,13 +995,13 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1006,13 +1009,13 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1020,13 +1023,13 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1034,13 +1037,13 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1048,13 +1051,13 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,13 +1065,13 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1076,13 +1079,13 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,13 +1093,13 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C34">
         <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,13 +1107,13 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C35">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1118,13 +1121,13 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C36">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,13 +1135,13 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,13 +1149,13 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,13 +1163,13 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1174,13 +1177,13 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C40">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,13 +1191,13 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C41">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,13 +1205,13 @@
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C42">
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,13 +1219,13 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C43">
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,13 +1233,13 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C44">
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1244,13 +1247,13 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C45">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,13 +1261,13 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C46">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,13 +1275,13 @@
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C47">
         <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,13 +1289,13 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C48">
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,13 +1303,13 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C49">
         <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,13 +1317,13 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C50">
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,13 +1331,13 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C51">
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,13 +1345,13 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C52">
         <v>9</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,13 +1359,13 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C53">
         <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,13 +1373,13 @@
         <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C54">
         <v>9</v>
       </c>
       <c r="D54" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,13 +1387,13 @@
         <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C55">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D55" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1398,13 +1401,13 @@
         <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C56">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D56" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1412,13 +1415,13 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C57">
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1426,13 +1429,13 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C58">
         <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,13 +1443,27 @@
         <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C59">
         <v>10</v>
       </c>
       <c r="D59" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>